<commit_message>
Added extra amphibole things, NNO, H2O, Zhang melt comps
</commit_message>
<xml_diff>
--- a/Machine_Learning_Phase_ID/KSpars_Shamloo.xlsx
+++ b/Machine_Learning_Phase_ID/KSpars_Shamloo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\penny\OneDrive - Oregon State University\Postdoc\PyMME\MyBarometers\Thermobar_outer\Machine_Learning_Phase_ID\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C37D62F1-5E7C-4BDD-910C-063E37356F8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B994A75E-2C40-449C-9E85-4DD4FBE382E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="21840" windowHeight="13290" xr2:uid="{D1CF62EB-CBE0-054B-BE72-B48AA9F2F7E8}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="21840" windowHeight="13290" activeTab="1" xr2:uid="{D1CF62EB-CBE0-054B-BE72-B48AA9F2F7E8}"/>
   </bookViews>
   <sheets>
     <sheet name="alkali feldspar_with_headings" sheetId="3" r:id="rId1"/>
@@ -3083,6 +3083,7 @@
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Cpx"/>
+      <sheetName val="To_Do"/>
       <sheetName val="Opx"/>
       <sheetName val="Plag"/>
       <sheetName val="Amp"/>
@@ -3096,15 +3097,16 @@
       <sheetName val="Ol"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7" refreshError="1"/>
-      <sheetData sheetId="8">
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9">
         <row r="1">
           <cell r="L1" t="str">
             <v>K2O_Kspar</v>
@@ -3951,9 +3953,9 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="9" refreshError="1"/>
-      <sheetData sheetId="10" refreshError="1"/>
-      <sheetData sheetId="11" refreshError="1"/>
+      <sheetData sheetId="10"/>
+      <sheetData sheetId="11"/>
+      <sheetData sheetId="12"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -4258,9 +4260,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4FE198C-A160-416C-A564-D1E9B6CBF185}">
   <dimension ref="A1:P697"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O1" sqref="O1"/>
+      <selection pane="bottomLeft" activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="15"/>
@@ -38430,9 +38432,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FED6DCF8-FC43-544A-8BE6-29532FE73FC4}">
   <dimension ref="A1:P697"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B697" sqref="B2:L697"/>
+      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="15"/>

</xml_diff>